<commit_message>
Started adding testing Started Cleaning up code Updated backlog Added Readme
</commit_message>
<xml_diff>
--- a/sprints/sprint1/Sprint Backlog .xlsx
+++ b/sprints/sprint1/Sprint Backlog .xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benev\Desktop\CS\Spring 2022\Capstone\Sprint1\sprints\sprint1\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0839CA4-E083-4B9B-9252-4F144FCCB853}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="4005" yWindow="915" windowWidth="22905" windowHeight="14685" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
   <si>
     <t>User Stories</t>
   </si>
@@ -85,30 +94,32 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
@@ -118,7 +129,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -134,108 +145,95 @@
     </fill>
   </fills>
   <borders count="2">
-    <border/>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="12">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="2">
     <dxf>
-      <font/>
       <fill>
-        <patternFill patternType="none"/>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF3F3F3"/>
+          <bgColor rgb="FFF3F3F3"/>
+        </patternFill>
       </fill>
-      <border/>
     </dxf>
     <dxf>
-      <font/>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFFFFFFF"/>
           <bgColor rgb="FFFFFFFF"/>
         </patternFill>
       </fill>
-      <border/>
-    </dxf>
-    <dxf>
-      <font/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF3F3F3"/>
-          <bgColor rgb="FFF3F3F3"/>
-        </patternFill>
-      </fill>
-      <border/>
     </dxf>
   </dxfs>
   <tableStyles count="1">
-    <tableStyle count="2" pivot="0" name="Sheet1-style">
-      <tableStyleElement dxfId="1" type="firstRowStripe"/>
-      <tableStyleElement dxfId="2" type="secondRowStripe"/>
+    <tableStyle name="Sheet1-style" pivot="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+      <tableStyleElement type="firstRowStripe" dxfId="1"/>
+      <tableStyleElement type="secondRowStripe" dxfId="0"/>
     </tableStyle>
   </tableStyles>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="A3:G10" displayName="Table_1" id="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A3:G10" headerRowCount="0">
   <tableColumns count="7">
-    <tableColumn name="Column1" id="1"/>
-    <tableColumn name="Column2" id="2"/>
-    <tableColumn name="Column3" id="3"/>
-    <tableColumn name="Column4" id="4"/>
-    <tableColumn name="Column5" id="5"/>
-    <tableColumn name="Column6" id="6"/>
-    <tableColumn name="Column7" id="7"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Column1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Column2"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Column3"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Column4"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Column5"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Column6"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Column7"/>
   </tableColumns>
-  <tableStyleInfo name="Sheet1-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+  <tableStyleInfo name="Sheet1-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -425,24 +423,29 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:U12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="2" width="41.14"/>
-    <col customWidth="1" min="3" max="3" width="22.71"/>
+    <col min="1" max="2" width="41.140625" customWidth="1"/>
+    <col min="3" max="3" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -475,7 +478,7 @@
       <c r="T1" s="3"/>
       <c r="U1" s="3"/>
     </row>
-    <row r="2">
+    <row r="2" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="5"/>
@@ -502,7 +505,7 @@
       <c r="T2" s="6"/>
       <c r="U2" s="6"/>
     </row>
-    <row r="3">
+    <row r="3" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>7</v>
       </c>
@@ -513,13 +516,13 @@
         <v>9</v>
       </c>
       <c r="D3" s="8">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="E3" s="8">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="F3" s="8">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G3" s="9"/>
       <c r="H3" s="10"/>
@@ -537,15 +540,23 @@
       <c r="T3" s="10"/>
       <c r="U3" s="10"/>
     </row>
-    <row r="4">
+    <row r="4" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
+      <c r="B4" s="7" t="s">
+        <v>8</v>
+      </c>
       <c r="C4" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
+      <c r="D4" s="9">
+        <v>4</v>
+      </c>
+      <c r="E4" s="9">
+        <v>2</v>
+      </c>
+      <c r="F4" s="9">
+        <v>0</v>
+      </c>
       <c r="G4" s="9"/>
       <c r="H4" s="10"/>
       <c r="I4" s="10"/>
@@ -562,7 +573,7 @@
       <c r="T4" s="10"/>
       <c r="U4" s="10"/>
     </row>
-    <row r="5">
+    <row r="5" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>11</v>
       </c>
@@ -573,13 +584,13 @@
         <v>13</v>
       </c>
       <c r="D5" s="8">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="E5" s="8">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="F5" s="8">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G5" s="9"/>
       <c r="H5" s="10"/>
@@ -597,15 +608,23 @@
       <c r="T5" s="10"/>
       <c r="U5" s="10"/>
     </row>
-    <row r="6">
+    <row r="6" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
+      <c r="B6" s="7" t="s">
+        <v>12</v>
+      </c>
       <c r="C6" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
+      <c r="D6" s="8">
+        <v>4</v>
+      </c>
+      <c r="E6" s="8">
+        <v>2</v>
+      </c>
+      <c r="F6" s="8">
+        <v>0</v>
+      </c>
       <c r="G6" s="9"/>
       <c r="H6" s="10"/>
       <c r="I6" s="10"/>
@@ -622,7 +641,7 @@
       <c r="T6" s="10"/>
       <c r="U6" s="10"/>
     </row>
-    <row r="7">
+    <row r="7" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>15</v>
       </c>
@@ -633,13 +652,13 @@
         <v>16</v>
       </c>
       <c r="D7" s="8">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="E7" s="8">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="F7" s="8">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G7" s="9"/>
       <c r="H7" s="10"/>
@@ -657,7 +676,7 @@
       <c r="T7" s="10"/>
       <c r="U7" s="10"/>
     </row>
-    <row r="8">
+    <row r="8" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>17</v>
       </c>
@@ -668,13 +687,13 @@
         <v>18</v>
       </c>
       <c r="D8" s="8">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="E8" s="8">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="F8" s="8">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="G8" s="9"/>
       <c r="H8" s="10"/>
@@ -692,7 +711,7 @@
       <c r="T8" s="10"/>
       <c r="U8" s="10"/>
     </row>
-    <row r="9">
+    <row r="9" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>19</v>
       </c>
@@ -703,13 +722,13 @@
         <v>21</v>
       </c>
       <c r="D9" s="8">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="E9" s="8">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="F9" s="8">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G9" s="9"/>
       <c r="H9" s="10"/>
@@ -727,15 +746,23 @@
       <c r="T9" s="10"/>
       <c r="U9" s="10"/>
     </row>
-    <row r="10">
+    <row r="10" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
+      <c r="B10" s="7" t="s">
+        <v>20</v>
+      </c>
       <c r="C10" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
+      <c r="D10" s="9">
+        <v>5</v>
+      </c>
+      <c r="E10" s="9">
+        <v>2</v>
+      </c>
+      <c r="F10" s="9">
+        <v>0</v>
+      </c>
       <c r="G10" s="9"/>
       <c r="H10" s="10"/>
       <c r="I10" s="10"/>
@@ -752,7 +779,7 @@
       <c r="T10" s="10"/>
       <c r="U10" s="10"/>
     </row>
-    <row r="11">
+    <row r="11" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="11"/>
       <c r="B11" s="11"/>
       <c r="C11" s="10"/>
@@ -775,7 +802,7 @@
       <c r="T11" s="10"/>
       <c r="U11" s="10"/>
     </row>
-    <row r="12">
+    <row r="12" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="11"/>
       <c r="B12" s="11"/>
       <c r="C12" s="10"/>
@@ -799,9 +826,9 @@
       <c r="U12" s="10"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>